<commit_message>
Fix dynamic gantt chart
</commit_message>
<xml_diff>
--- a/ExampleFiles/tasks.xlsx
+++ b/ExampleFiles/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1387C0C7-866D-4B15-8C84-3BBF7D3F5F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC05C53E-46B5-4171-AC2D-472B5737718E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -369,7 +369,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -397,7 +397,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -408,7 +408,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -430,7 +430,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add 2 gantt charts in the same page, still to be changed to reflect multiple dimensions, task, and project
</commit_message>
<xml_diff>
--- a/ExampleFiles/tasks.xlsx
+++ b/ExampleFiles/tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC05C53E-46B5-4171-AC2D-472B5737718E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C86AEB-4E18-4ECA-A8B9-ACA230E19409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Task Name</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
+  </si>
+  <si>
+    <t>Progress</t>
   </si>
 </sst>
 </file>
@@ -366,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -378,7 +384,7 @@
     <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -388,8 +394,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -399,8 +411,11 @@
       <c r="C2">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -410,8 +425,11 @@
       <c r="C3">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -421,8 +439,11 @@
       <c r="C4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -433,7 +454,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -442,6 +463,9 @@
       </c>
       <c r="C6">
         <v>50</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix gantt from files
</commit_message>
<xml_diff>
--- a/ExampleFiles/tasks.xlsx
+++ b/ExampleFiles/tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josef\source\repos\SpreadsheetUtilities\ExampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1861CEF2-FD86-419B-9172-324032937135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5A83BF8-6003-4B37-8B56-4453E843E375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11352" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,6 +127,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0">
   <autoFilter ref="A1:H6" xr:uid="{CA36BCF6-9D3D-4FB5-B989-1CE0C17CF698}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H6">
+    <sortCondition descending="1" ref="E1:E6"/>
+  </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{C11070B8-C7FE-4695-859A-8CFBC6660079}" name="ID"/>
     <tableColumn id="7" xr3:uid="{0D440719-8745-4E73-9729-B73B2CC0C00E}" name="ProjectID"/>
@@ -406,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,24 +472,27 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>55</v>
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -495,18 +501,15 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4">
-        <v>15</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -515,10 +518,13 @@
         <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>60</v>
+        <v>50</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -526,25 +532,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
         <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6">
-        <v>50</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>